<commit_message>
EPBDS-8950 Fields with default value should be nillable. Fix a condition.
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebServiceAnnotation/openl-repository/deployments/ws-annotation/ws-annotation/MAIN-20181121.xlsx
+++ b/ITEST/itest.WebServiceAnnotation/openl-repository/deployments/ws-annotation/ws-annotation/MAIN-20181121.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563916B0-25EB-4325-89C6-01E0D571E6CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95140A6F-BA00-4B9E-B5CC-B7FAA2F15B44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="810" windowWidth="21495" windowHeight="18375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5910" yWindow="1620" windowWidth="28875" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Step</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Spreadsheet Integer parse6(String str)</t>
+  </si>
+  <si>
+    <t>0.0</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="C4:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,12 +741,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>0</v>
       </c>
@@ -751,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>2</v>
       </c>
@@ -759,12 +762,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>31</v>
       </c>
@@ -772,20 +775,23 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>34</v>
       </c>
       <c r="D59" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
QueryParam is ignored in REST service interface
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebServiceAnnotation/openl-repository/deployments/ws-annotation/ws-annotation/MAIN-20181121.xlsx
+++ b/ITEST/itest.WebServiceAnnotation/openl-repository/deployments/ws-annotation/ws-annotation/MAIN-20181121.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95140A6F-BA00-4B9E-B5CC-B7FAA2F15B44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF058C1-464B-4956-A55E-D44D6AA48695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="1620" windowWidth="28875" windowHeight="17610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Step</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>0.0</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer parse4QueryParam(String str)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Integer parse4PathParam(String str)</t>
   </si>
 </sst>
 </file>
@@ -526,16 +532,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:K81"/>
+  <dimension ref="C4:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -686,187 +692,229 @@
         <v>13</v>
       </c>
     </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>37</v>
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D46" s="1" t="s">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="1" t="s">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
         <v>31</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D64" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>34</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D65" t="s">
         <v>33</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E65" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="1" t="s">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70" s="1" t="s">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>2</v>
-      </c>
-      <c r="D81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>